<commit_message>
change version to 0.1.0
</commit_message>
<xml_diff>
--- a/examples/complex.xlsx
+++ b/examples/complex.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="JS XLSX"/>
   <workbookPr showObjects="all"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
-  <calcPr iterateCount="100" iterate="false" iterateDelta="0.001" refMode="A1"/>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1" state="visible"/>
   </sheets>
+  <calcPr iterateCount="100" iterate="0" iterateDelta="0.001" refMode="A1"/>
 </workbook>
 </file>
 
@@ -177,13 +177,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
-    <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-    </border>
+  <borders count="2">
     <border>
       <left style="none"/>
       <right style="none"/>
@@ -205,31 +199,26 @@
       </bottom>
     </border>
   </borders>
-  <cellStyleXfs/>
-  <cellXfs count="7">
-    <xf>
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+  <cellXfs count="6">
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" applyBorder="false" applyFill="false" applyFont="false" applyAlignment="false" fontId="0" fillId="0" borderId="1">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="1" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" applyBorder="false" applyFill="false" applyFont="false" applyAlignment="false" fontId="1" fillId="2" borderId="2">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="3" fontId="1" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" applyBorder="false" applyFill="false" applyFont="false" applyAlignment="false" fontId="1" fillId="3" borderId="2">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="4" fontId="1" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" applyBorder="false" applyFill="false" applyFont="false" applyAlignment="false" fontId="1" fillId="4" borderId="2">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="1" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" applyBorder="false" applyFill="false" applyFont="false" applyAlignment="false" fontId="1" fillId="0" borderId="2">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-    </xf>
-    <xf numFmtId="0" applyBorder="false" applyFill="false" applyFont="false" applyAlignment="false" fontId="1" fillId="5" borderId="2">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="5" fontId="1" numFmtId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
-  <numFmts/>
 </styleSheet>
 </file>
 
@@ -555,184 +544,184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+  <sheetPr filterMode="0">
+    <pageSetUpPr fitToPage="0"/>
   </sheetPr>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="1" rightToLeft="0" showFormulas="0" showGridLines="1" showOutlineSymbols="1" showRowColHeaders="1" showZeros="1" tabSelected="1" topLeftCell="A1" view="normal" windowProtection="0" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85" defaultColWidth="0"/>
-  <printOptions gridLines="false" gridLinesSet="true" headings="false" horizontalCentered="false" verticalCentered="false"/>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col min="1" max="1" hidden="0" width="11.4" customWidth="1" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="2" max="2" hidden="0" width="11.8" customWidth="1" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="3" max="3" hidden="0" width="11.7" customWidth="1" collapsed="0" outlineLevel="0" style="0"/>
+    <col min="4" max="4" hidden="0" width="11.8" customWidth="1" collapsed="0" outlineLevel="0" style="0"/>
+  </cols>
+  <sheetData>
+    <row r="1" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A1" t="s" s="1">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s" s="1">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A2" t="s" s="2">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s" s="4">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s" s="4">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A3" t="s" s="2">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s" s="5">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A4" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s" s="3">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s" s="4">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s" s="4">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A5" t="s" s="2">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s" s="5">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s" s="5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A6" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="B6" t="s" s="3">
+        <v>20</v>
+      </c>
+      <c r="C6" t="s" s="4">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s" s="4">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A7" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="B7" t="s" s="3">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s" s="5">
+        <v>24</v>
+      </c>
+      <c r="D7" t="s" s="5">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A8" t="s" s="2">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s" s="3">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s" s="4">
+        <v>12</v>
+      </c>
+      <c r="D8" t="s" s="4">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A9" t="s" s="2">
+        <v>29</v>
+      </c>
+      <c r="B9" t="s" s="3">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s" s="5">
+        <v>20</v>
+      </c>
+      <c r="D9" t="s" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A10" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s" s="3">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s" s="4">
+        <v>31</v>
+      </c>
+      <c r="D10" t="s" s="4">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" customHeight="1" ht="20.00125984752" outlineLevel="0">
+      <c r="A11" t="s" s="4">
+        <v>33</v>
+      </c>
+      <c r="B11" t="s" s="4">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s" s="4">
+        <v>35</v>
+      </c>
+      <c r="D11" t="s" s="4">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup blackAndWhite="false" cellComments="none" copies="1" draft="false" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="true" usePrinterDefaults="false" verticalDpi="300"/>
+  <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <dimension ref="A1:D11"/>
-  <cols>
-    <col min="1" max="1" hidden="false" width="11.4" customWidth="1" collapsed="false" outlineLevel="0" style="1"/>
-    <col min="2" max="2" hidden="false" width="11.8" customWidth="1" collapsed="false" outlineLevel="0" style="1"/>
-    <col min="3" max="3" hidden="false" width="11.7" customWidth="1" collapsed="false" outlineLevel="0" style="1"/>
-    <col min="4" max="4" hidden="false" width="11.8" customWidth="1" collapsed="false" outlineLevel="0" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s" s="2">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s" s="2">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A2" t="s" s="3">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s" s="5">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s" s="5">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A3" t="s" s="3">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s" s="6">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s" s="6">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A4" t="s" s="3">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s" s="4">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s" s="5">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s" s="5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A5" t="s" s="3">
-        <v>15</v>
-      </c>
-      <c r="B5" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s" s="6">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s" s="6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A6" t="s" s="3">
-        <v>19</v>
-      </c>
-      <c r="B6" t="s" s="4">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s" s="5">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s" s="5">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A7" t="s" s="3">
-        <v>23</v>
-      </c>
-      <c r="B7" t="s" s="4">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s" s="6">
-        <v>24</v>
-      </c>
-      <c r="D7" t="s" s="6">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="8" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A8" t="s" s="3">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s" s="4">
-        <v>27</v>
-      </c>
-      <c r="C8" t="s" s="5">
-        <v>12</v>
-      </c>
-      <c r="D8" t="s" s="5">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A9" t="s" s="3">
-        <v>29</v>
-      </c>
-      <c r="B9" t="s" s="4">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s" s="6">
-        <v>20</v>
-      </c>
-      <c r="D9" t="s" s="6">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A10" t="s" s="3">
-        <v>30</v>
-      </c>
-      <c r="B10" t="s" s="4">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s" s="5">
-        <v>31</v>
-      </c>
-      <c r="D10" t="s" s="5">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" customHeight="true" ht="20.00125984752" outlineLevel="0">
-      <c r="A11" t="s" s="5">
-        <v>33</v>
-      </c>
-      <c r="B11" t="s" s="5">
-        <v>34</v>
-      </c>
-      <c r="C11" t="s" s="5">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s" s="5">
-        <v>36</v>
-      </c>
-    </row>
-  </sheetData>
 </worksheet>
 </file>
</xml_diff>